<commit_message>
Add CONLL, Close #1
</commit_message>
<xml_diff>
--- a/2018-CFP-NLP.xlsx
+++ b/2018-CFP-NLP.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="252">
   <si>
     <t>page</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -260,10 +260,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2018.06.03</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Melbourne, Australia</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -337,10 +333,6 @@
   </si>
   <si>
     <t>CIKM</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TBD</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1029,10 +1021,6 @@
     <t>https://conference.cs.cityu.edu.hk/iconip/</t>
   </si>
   <si>
-    <t>比利时</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>2018.02.11</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1050,6 +1038,29 @@
   </si>
   <si>
     <t>2018.05.18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2018.06.01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2018.07.27</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2018.10.31</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Brussels, Belgium</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rio de Janeiro, Brazil</t>
+  </si>
+  <si>
+    <t>2018.07.08</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1057,7 +1068,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1172,13 +1183,6 @@
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF3E3E3E"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1300,7 +1304,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1365,6 +1369,12 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1382,15 +1392,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1703,10 +1704,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G12" sqref="A1:I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1724,18 +1725,18 @@
   <sheetData>
     <row r="1" spans="1:9" s="10" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="B1" s="9" t="s">
-        <v>145</v>
-      </c>
       <c r="C1" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="29" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="9" t="s">
@@ -1753,109 +1754,109 @@
     </row>
     <row r="2" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C2" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" s="28" t="s">
         <v>83</v>
-      </c>
-      <c r="E2" s="34" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="E3" s="34" t="s">
-        <v>158</v>
+        <v>155</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>156</v>
       </c>
       <c r="I3" s="23" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>159</v>
-      </c>
-      <c r="E4" s="34" t="s">
-        <v>160</v>
+        <v>157</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>158</v>
       </c>
       <c r="I4" s="23" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C5" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" s="28" t="s">
         <v>95</v>
-      </c>
-      <c r="E5" s="34" t="s">
-        <v>97</v>
       </c>
       <c r="I5" s="23"/>
     </row>
     <row r="6" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="E6" s="28" t="s">
         <v>98</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="E6" s="34" t="s">
-        <v>100</v>
       </c>
       <c r="I6" s="23"/>
     </row>
     <row r="7" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C7" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="E7" s="28" t="s">
         <v>84</v>
-      </c>
-      <c r="E7" s="34" t="s">
-        <v>86</v>
       </c>
       <c r="I7" s="23"/>
     </row>
     <row r="8" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="E8" s="34" t="s">
-        <v>85</v>
+      <c r="E8" s="28" t="s">
+        <v>83</v>
       </c>
       <c r="F8" s="10" t="s">
         <v>23</v>
@@ -1867,30 +1868,30 @@
         <v>47</v>
       </c>
       <c r="I8" s="23" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="E9" s="34" t="s">
-        <v>85</v>
+      <c r="E9" s="28" t="s">
+        <v>83</v>
       </c>
       <c r="F9" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="G9" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="H9" s="13" t="s">
         <v>65</v>
-      </c>
-      <c r="H9" s="13" t="s">
-        <v>66</v>
       </c>
       <c r="I9" s="23" t="s">
         <v>51</v>
@@ -1898,62 +1899,62 @@
     </row>
     <row r="10" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>109</v>
-      </c>
-      <c r="E10" s="34" t="s">
-        <v>226</v>
+        <v>107</v>
+      </c>
+      <c r="E10" s="28" t="s">
+        <v>224</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I10" s="23" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="E11" s="34" t="s">
+      <c r="E11" s="28" t="s">
         <v>56</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>57</v>
+        <v>251</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>58</v>
+        <v>250</v>
       </c>
       <c r="I11" s="23" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>14</v>
@@ -1961,112 +1962,112 @@
       <c r="D12" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="34" t="s">
-        <v>59</v>
+      <c r="E12" s="28" t="s">
+        <v>58</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="G12" s="10" t="s">
         <v>54</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I12" s="23" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="34" t="s">
-        <v>62</v>
+      <c r="E13" s="28" t="s">
+        <v>61</v>
       </c>
       <c r="F13" s="10" t="s">
         <v>22</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H13" s="13" t="s">
         <v>50</v>
       </c>
       <c r="I13" s="23" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="E14" s="34" t="s">
-        <v>104</v>
+        <v>101</v>
+      </c>
+      <c r="E14" s="28" t="s">
+        <v>102</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="I14" s="23" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="E15" s="34" t="s">
-        <v>244</v>
+        <v>105</v>
+      </c>
+      <c r="E15" s="28" t="s">
+        <v>241</v>
       </c>
       <c r="F15" s="21" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="I15" s="13" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C16" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="E16" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="E16" s="34" t="s">
+      <c r="F16" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="G16" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="G16" s="10" t="s">
-        <v>70</v>
-      </c>
       <c r="H16" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I16" s="23" t="s">
         <v>52</v>
@@ -2074,270 +2075,279 @@
     </row>
     <row r="17" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C17" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="E17" s="14" t="s">
         <v>71</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>72</v>
       </c>
       <c r="F17" s="10" t="s">
         <v>46</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I17" s="23" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D18" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>243</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="H18" s="13" t="s">
         <v>238</v>
       </c>
-      <c r="E18" s="14" t="s">
-        <v>246</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>239</v>
-      </c>
-      <c r="H18" s="13" t="s">
-        <v>240</v>
-      </c>
       <c r="I18" s="23" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="I19" s="23"/>
     </row>
     <row r="20" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E20" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="G20" s="10" t="s">
         <v>231</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="H20" s="13" t="s">
         <v>232</v>
       </c>
-      <c r="G20" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="H20" s="13" t="s">
-        <v>234</v>
-      </c>
       <c r="I20" s="23" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="I21" s="23" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D22" s="10" t="s">
         <v>49</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H22" s="13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I22" s="23" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E23" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="G23" s="10" t="s">
         <v>227</v>
       </c>
-      <c r="F23" s="10" t="s">
-        <v>228</v>
-      </c>
-      <c r="G23" s="10" t="s">
-        <v>229</v>
-      </c>
-      <c r="H23" s="35" t="s">
-        <v>243</v>
+      <c r="H23" s="13" t="s">
+        <v>249</v>
       </c>
       <c r="I23" s="23" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>115</v>
+        <v>74</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>65</v>
+        <v>246</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>237</v>
+        <v>247</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>248</v>
       </c>
       <c r="H24" s="13" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="I24" s="23" t="s">
-        <v>242</v>
+        <v>171</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="13"/>
-      <c r="B25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="I25" s="13"/>
+      <c r="A25" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="I25" s="23" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="26" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C26" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="E26" s="14" t="s">
         <v>112</v>
-      </c>
-      <c r="E26" s="14" t="s">
-        <v>114</v>
       </c>
       <c r="I26" s="23"/>
     </row>
     <row r="27" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>75</v>
+        <v>106</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="H27" s="35"/>
+        <v>104</v>
+      </c>
       <c r="I27" s="23" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="B28" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="C28" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="E28" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="I28" s="23" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="13"/>
+      <c r="B29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+      <c r="I29" s="13"/>
+    </row>
     <row r="30" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="13"/>
-      <c r="B30" s="13"/>
+      <c r="B30" s="11" t="s">
+        <v>145</v>
+      </c>
       <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
+      <c r="E30" s="17"/>
       <c r="F30" s="13"/>
       <c r="G30" s="13"/>
       <c r="I30" s="13"/>
     </row>
     <row r="31" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="11" t="s">
-        <v>147</v>
+      <c r="B31" s="18" t="s">
+        <v>146</v>
       </c>
       <c r="D31" s="13"/>
       <c r="E31" s="17"/>
@@ -2346,8 +2356,8 @@
       <c r="I31" s="13"/>
     </row>
     <row r="32" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="18" t="s">
-        <v>148</v>
+      <c r="B32" s="19" t="s">
+        <v>147</v>
       </c>
       <c r="D32" s="13"/>
       <c r="E32" s="17"/>
@@ -2356,8 +2366,8 @@
       <c r="I32" s="13"/>
     </row>
     <row r="33" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="19" t="s">
-        <v>149</v>
+      <c r="B33" s="11" t="s">
+        <v>144</v>
       </c>
       <c r="D33" s="13"/>
       <c r="E33" s="17"/>
@@ -2366,62 +2376,88 @@
       <c r="I33" s="13"/>
     </row>
     <row r="34" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="D34" s="13"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
+      <c r="B34" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="C34" s="20"/>
       <c r="I34" s="13"/>
     </row>
     <row r="35" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="C35" s="20"/>
+        <v>175</v>
+      </c>
       <c r="I35" s="13"/>
     </row>
     <row r="36" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="23" t="s">
-        <v>177</v>
+        <v>151</v>
       </c>
       <c r="I36" s="13"/>
     </row>
     <row r="37" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="23" t="s">
-        <v>153</v>
-      </c>
-      <c r="I37" s="13"/>
+      <c r="B37" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="C37" s="22"/>
+      <c r="D37" s="23" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="38" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="18" t="s">
-        <v>161</v>
-      </c>
-      <c r="C38" s="22"/>
+        <v>160</v>
+      </c>
       <c r="D38" s="23" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="39" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="18" t="s">
-        <v>162</v>
-      </c>
-      <c r="D39" s="23" t="s">
-        <v>151</v>
-      </c>
-    </row>
+        <v>149</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="40" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="41" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="42" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="43" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="2:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B35:B37">
+  <conditionalFormatting sqref="B34:B36">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D37:D38">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A25:I27 A23:G24 A15:C15 A1:I2 A3:A4 C3:I4 A5:I14 I3:I14 I22:I24 E15:H15 A16:I22">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H24">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -2433,20 +2469,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D38:D39">
+  <conditionalFormatting sqref="H23">
     <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A28:I28 A27:G27 A24:I24 A26:I26 A23:G23 A15:C15 A1:I2 A3:A4 C3:I4 A5:I14 I3:I14 I27 I22:I23 E15:H15 A16:I22">
-    <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2465,15 +2489,15 @@
     <hyperlink ref="I16" r:id="rId5"/>
     <hyperlink ref="I22" r:id="rId6"/>
     <hyperlink ref="I20" r:id="rId7"/>
-    <hyperlink ref="I28" r:id="rId8"/>
+    <hyperlink ref="I27" r:id="rId8"/>
     <hyperlink ref="I11" r:id="rId9"/>
     <hyperlink ref="I18" r:id="rId10"/>
-    <hyperlink ref="I27" r:id="rId11"/>
-    <hyperlink ref="B35" r:id="rId12"/>
-    <hyperlink ref="B36" r:id="rId13"/>
-    <hyperlink ref="B37" r:id="rId14" location="/"/>
-    <hyperlink ref="D38" r:id="rId15"/>
-    <hyperlink ref="D39" r:id="rId16"/>
+    <hyperlink ref="I24" r:id="rId11"/>
+    <hyperlink ref="B34" r:id="rId12"/>
+    <hyperlink ref="B35" r:id="rId13"/>
+    <hyperlink ref="B36" r:id="rId14" location="/"/>
+    <hyperlink ref="D37" r:id="rId15"/>
+    <hyperlink ref="D38" r:id="rId16"/>
     <hyperlink ref="I23" r:id="rId17"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2745,266 +2769,266 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
+        <v>177</v>
+      </c>
+      <c r="B1" s="24" t="s">
         <v>179</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="C1" s="24" t="s">
+        <v>178</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="30" t="s">
+        <v>180</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>182</v>
+      </c>
+      <c r="C2" s="25" t="s">
         <v>181</v>
       </c>
-      <c r="C1" s="24" t="s">
-        <v>180</v>
-      </c>
-      <c r="D1" s="27" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="28" t="s">
+    </row>
+    <row r="3" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="31"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="25" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="31"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="25" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="31"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="25" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="31"/>
+      <c r="B6" s="26" t="s">
+        <v>187</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="31"/>
+      <c r="B7" s="26" t="s">
         <v>182</v>
       </c>
-      <c r="B2" s="31" t="s">
-        <v>184</v>
-      </c>
-      <c r="C2" s="25" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="29"/>
-      <c r="B3" s="32"/>
-      <c r="C3" s="25" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="29"/>
-      <c r="B4" s="32"/>
-      <c r="C4" s="25" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="29"/>
-      <c r="B5" s="33"/>
-      <c r="C5" s="25" t="s">
+      <c r="C7" s="25" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="31"/>
+      <c r="B8" s="26" t="s">
+        <v>190</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="41.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="31"/>
+      <c r="B9" s="26" t="s">
+        <v>182</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="32"/>
+      <c r="B10" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="30" t="s">
+        <v>194</v>
+      </c>
+      <c r="B11" s="33" t="s">
+        <v>182</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="31"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="25" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="31"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="25" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="31"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="25" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="32"/>
+      <c r="B15" s="26" t="s">
+        <v>200</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="30" t="s">
+        <v>201</v>
+      </c>
+      <c r="B16" s="33" t="s">
+        <v>203</v>
+      </c>
+      <c r="C16" s="25" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="31"/>
+      <c r="B17" s="35"/>
+      <c r="C17" s="25" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="31"/>
+      <c r="B18" s="33" t="s">
+        <v>203</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="31"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="25" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="31"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="25" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="31"/>
+      <c r="B21" s="35"/>
+      <c r="C21" s="25" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="31"/>
+      <c r="B22" s="26" t="s">
+        <v>182</v>
+      </c>
+      <c r="C22" s="25" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="32"/>
+      <c r="B23" s="26" t="s">
+        <v>200</v>
+      </c>
+      <c r="C23" s="25" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="30" t="s">
+        <v>211</v>
+      </c>
+      <c r="B24" s="33" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="29"/>
-      <c r="B6" s="26" t="s">
-        <v>189</v>
-      </c>
-      <c r="C6" s="25" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="29"/>
-      <c r="B7" s="26" t="s">
-        <v>184</v>
-      </c>
-      <c r="C7" s="25" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="29"/>
-      <c r="B8" s="26" t="s">
-        <v>192</v>
-      </c>
-      <c r="C8" s="25" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="41.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="29"/>
-      <c r="B9" s="26" t="s">
-        <v>184</v>
-      </c>
-      <c r="C9" s="25" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="30"/>
-      <c r="B10" s="26" t="s">
-        <v>195</v>
-      </c>
-      <c r="C10" s="25" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="28" t="s">
-        <v>196</v>
-      </c>
-      <c r="B11" s="31" t="s">
-        <v>184</v>
-      </c>
-      <c r="C11" s="25" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="29"/>
-      <c r="B12" s="32"/>
-      <c r="C12" s="25" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="29"/>
-      <c r="B13" s="32"/>
-      <c r="C13" s="25" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="29"/>
-      <c r="B14" s="33"/>
-      <c r="C14" s="25" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="30"/>
-      <c r="B15" s="26" t="s">
-        <v>202</v>
-      </c>
-      <c r="C15" s="25" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="28" t="s">
+      <c r="C24" s="25" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="31"/>
+      <c r="B25" s="34"/>
+      <c r="C25" s="25" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="31"/>
+      <c r="B26" s="35"/>
+      <c r="C26" s="25" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="31"/>
+      <c r="B27" s="33" t="s">
         <v>203</v>
       </c>
-      <c r="B16" s="31" t="s">
-        <v>205</v>
-      </c>
-      <c r="C16" s="25" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="29"/>
-      <c r="B17" s="33"/>
-      <c r="C17" s="25" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="29"/>
-      <c r="B18" s="31" t="s">
-        <v>205</v>
-      </c>
-      <c r="C18" s="25" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="29"/>
-      <c r="B19" s="32"/>
-      <c r="C19" s="25" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="29"/>
-      <c r="B20" s="32"/>
-      <c r="C20" s="25" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="29"/>
-      <c r="B21" s="33"/>
-      <c r="C21" s="25" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="29"/>
-      <c r="B22" s="26" t="s">
-        <v>184</v>
-      </c>
-      <c r="C22" s="25" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="30"/>
-      <c r="B23" s="26" t="s">
-        <v>202</v>
-      </c>
-      <c r="C23" s="25" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="28" t="s">
-        <v>213</v>
-      </c>
-      <c r="B24" s="31" t="s">
-        <v>189</v>
-      </c>
-      <c r="C24" s="25" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="29"/>
-      <c r="B25" s="32"/>
-      <c r="C25" s="25" t="s">
+      <c r="C27" s="25" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="29"/>
-      <c r="B26" s="33"/>
-      <c r="C26" s="25" t="s">
+    <row r="28" spans="1:3" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="31"/>
+      <c r="B28" s="34"/>
+      <c r="C28" s="25" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="29"/>
-      <c r="B27" s="31" t="s">
-        <v>205</v>
-      </c>
-      <c r="C27" s="25" t="s">
+    <row r="29" spans="1:3" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="31"/>
+      <c r="B29" s="35"/>
+      <c r="C29" s="25" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="29"/>
-      <c r="B28" s="32"/>
-      <c r="C28" s="25" t="s">
+    <row r="30" spans="1:3" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="31"/>
+      <c r="B30" s="26" t="s">
+        <v>187</v>
+      </c>
+      <c r="C30" s="25" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="29"/>
-      <c r="B29" s="33"/>
-      <c r="C29" s="25" t="s">
+    <row r="31" spans="1:3" ht="41.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="32"/>
+      <c r="B31" s="26" t="s">
+        <v>220</v>
+      </c>
+      <c r="C31" s="25" t="s">
         <v>219</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="27.75" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="29"/>
-      <c r="B30" s="26" t="s">
-        <v>189</v>
-      </c>
-      <c r="C30" s="25" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="41.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="30"/>
-      <c r="B31" s="26" t="s">
-        <v>222</v>
-      </c>
-      <c r="C31" s="25" t="s">
-        <v>221</v>
       </c>
     </row>
   </sheetData>

</xml_diff>